<commit_message>
Update Excel Dia 13/10
</commit_message>
<xml_diff>
--- a/Informativos/Aulas_Links_e_Datas_de_Exercícios.xlsx
+++ b/Informativos/Aulas_Links_e_Datas_de_Exercícios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Documents\GitHub\Segundo-Semestre-unip\Informativos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095D7869-DC89-4E50-9265-03078D6E3EE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740A97B1-DEE4-4EDD-A1B2-83A1E5FC1A32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2B392B0C-D6AE-496D-B771-9E3827DB5614}"/>
   </bookViews>
@@ -830,7 +830,7 @@
   <dimension ref="A1:W27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="O3" sqref="O2:O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.15"/>
@@ -838,8 +838,8 @@
     <col min="1" max="1" width="40" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" customWidth="1"/>
-    <col min="6" max="6" width="27.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" customWidth="1"/>
+    <col min="6" max="6" width="28.6640625" customWidth="1"/>
     <col min="11" max="11" width="9.33203125" customWidth="1"/>
     <col min="16" max="23" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -955,10 +955,10 @@
       <c r="M2" s="10">
         <v>44102</v>
       </c>
-      <c r="N2" s="14">
+      <c r="N2" s="10">
         <v>44109</v>
       </c>
-      <c r="O2" s="15">
+      <c r="O2" s="13">
         <v>44116</v>
       </c>
       <c r="P2" s="14">
@@ -1022,10 +1022,10 @@
       <c r="M3" s="10">
         <v>44102</v>
       </c>
-      <c r="N3" s="14">
+      <c r="N3" s="10">
         <v>44109</v>
       </c>
-      <c r="O3" s="15">
+      <c r="O3" s="13">
         <v>44116</v>
       </c>
       <c r="P3" s="14">
@@ -1090,13 +1090,13 @@
       <c r="L4" s="13">
         <v>44096</v>
       </c>
-      <c r="M4" s="14">
+      <c r="M4" s="2">
         <v>44103</v>
       </c>
       <c r="N4" s="13">
         <v>44110</v>
       </c>
-      <c r="O4" s="14">
+      <c r="O4" s="2">
         <v>44117</v>
       </c>
       <c r="P4" s="13">
@@ -1157,13 +1157,13 @@
       <c r="L5" s="13">
         <v>44096</v>
       </c>
-      <c r="M5" s="14">
+      <c r="M5" s="2">
         <v>44103</v>
       </c>
       <c r="N5" s="13">
         <v>44110</v>
       </c>
-      <c r="O5" s="14">
+      <c r="O5" s="2">
         <v>44117</v>
       </c>
       <c r="P5" s="13">
@@ -1229,10 +1229,10 @@
       <c r="M6" s="13">
         <v>44103</v>
       </c>
-      <c r="N6" s="14">
+      <c r="N6" s="2">
         <v>44110</v>
       </c>
-      <c r="O6" s="13">
+      <c r="O6" s="16">
         <v>44117</v>
       </c>
       <c r="P6" s="14">
@@ -1296,10 +1296,10 @@
       <c r="M7" s="13">
         <v>44103</v>
       </c>
-      <c r="N7" s="14">
+      <c r="N7" s="2">
         <v>44110</v>
       </c>
-      <c r="O7" s="13">
+      <c r="O7" s="16">
         <v>44117</v>
       </c>
       <c r="P7" s="14">
@@ -1364,10 +1364,10 @@
       <c r="L8" s="2">
         <v>44097</v>
       </c>
-      <c r="M8" s="16">
+      <c r="M8" s="2">
         <v>44104</v>
       </c>
-      <c r="N8" s="14">
+      <c r="N8" s="2">
         <v>44111</v>
       </c>
       <c r="O8" s="14">
@@ -1420,25 +1420,25 @@
       <c r="G9" s="2">
         <v>44062</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="10">
         <v>44069</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="10">
         <v>44076</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="10">
         <v>44083</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="10">
         <v>44090</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L9" s="10">
         <v>44097</v>
       </c>
-      <c r="M9" s="16">
+      <c r="M9" s="10">
         <v>44104</v>
       </c>
-      <c r="N9" s="14">
+      <c r="N9" s="10">
         <v>44111</v>
       </c>
       <c r="O9" s="14">
@@ -1506,10 +1506,10 @@
       <c r="L10" s="2">
         <v>44098</v>
       </c>
-      <c r="M10" s="14">
+      <c r="M10" s="2">
         <v>44105</v>
       </c>
-      <c r="N10" s="14">
+      <c r="N10" s="2">
         <v>44112</v>
       </c>
       <c r="O10" s="14">
@@ -1573,10 +1573,10 @@
       <c r="L11" s="2">
         <v>44098</v>
       </c>
-      <c r="M11" s="14">
+      <c r="M11" s="2">
         <v>44105</v>
       </c>
-      <c r="N11" s="14">
+      <c r="N11" s="2">
         <v>44112</v>
       </c>
       <c r="O11" s="14">
@@ -1635,19 +1635,19 @@
       <c r="I12" s="13">
         <v>44078</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="10">
         <v>44085</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12" s="10">
         <v>44092</v>
       </c>
-      <c r="L12" s="2">
+      <c r="L12" s="10">
         <v>44099</v>
       </c>
-      <c r="M12" s="6">
+      <c r="M12" s="10">
         <v>44106</v>
       </c>
-      <c r="N12" s="6">
+      <c r="N12" s="10">
         <v>44113</v>
       </c>
       <c r="O12" s="6">
@@ -1706,19 +1706,19 @@
       <c r="I13" s="13">
         <v>44078</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="10">
         <v>44085</v>
       </c>
       <c r="K13" s="10">
         <v>44092</v>
       </c>
-      <c r="L13" s="2">
+      <c r="L13" s="10">
         <v>44099</v>
       </c>
-      <c r="M13" s="6">
+      <c r="M13" s="10">
         <v>44106</v>
       </c>
-      <c r="N13" s="6">
+      <c r="N13" s="10">
         <v>44113</v>
       </c>
       <c r="O13" s="6">

</xml_diff>

<commit_message>
LPA Completo EX e LAB
</commit_message>
<xml_diff>
--- a/Informativos/Aulas_Links_e_Datas_de_Exercícios.xlsx
+++ b/Informativos/Aulas_Links_e_Datas_de_Exercícios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Documents\GitHub\Segundo-Semestre-unip\Informativos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740A97B1-DEE4-4EDD-A1B2-83A1E5FC1A32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB4BE76-79B4-4C8C-9F20-FC70178C0849}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2B392B0C-D6AE-496D-B771-9E3827DB5614}"/>
   </bookViews>
@@ -830,7 +830,7 @@
   <dimension ref="A1:W27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O2:O3"/>
+      <selection activeCell="H10" sqref="G10:N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.15"/>
@@ -1346,28 +1346,28 @@
       <c r="F8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="10">
         <v>44062</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="10">
         <v>44069</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="10">
         <v>44076</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="10">
         <v>44083</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="10">
         <v>44090</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8" s="10">
         <v>44097</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M8" s="10">
         <v>44104</v>
       </c>
-      <c r="N8" s="2">
+      <c r="N8" s="10">
         <v>44111</v>
       </c>
       <c r="O8" s="14">
@@ -1417,7 +1417,7 @@
       <c r="F9" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="10">
         <v>44062</v>
       </c>
       <c r="H9" s="10">

</xml_diff>